<commit_message>
Added test case screenshots and linked them in Excel file
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\junie\QA-Test-Plan-AutomationExcercise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EAE42E2B-5B2B-4967-B881-2DA0CE240E4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD4EA2DE-B16E-4C6B-8A86-524CBBA2F020}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12156" yWindow="1440" windowWidth="9324" windowHeight="8880" xr2:uid="{B8137427-FE0E-4218-AA7C-363CA8DBE690}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B8137427-FE0E-4218-AA7C-363CA8DBE690}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,9 +35,185 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="57">
+  <si>
+    <t>Test ID</t>
+  </si>
+  <si>
+    <t>Features</t>
+  </si>
+  <si>
+    <t>Test Scenario</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>Actual Result</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Screenshot Reference</t>
+  </si>
+  <si>
+    <t>TC01</t>
+  </si>
+  <si>
+    <t>TC02</t>
+  </si>
+  <si>
+    <t>TC03</t>
+  </si>
+  <si>
+    <t>TC04</t>
+  </si>
+  <si>
+    <t>TC05</t>
+  </si>
+  <si>
+    <t>TC06</t>
+  </si>
+  <si>
+    <t>TC07</t>
+  </si>
+  <si>
+    <t>TC08</t>
+  </si>
+  <si>
+    <t>Homepage</t>
+  </si>
+  <si>
+    <t>Verify homepage loads with correct title/logo</t>
+  </si>
+  <si>
+    <t>Homepage displays title/logo correctly</t>
+  </si>
+  <si>
+    <t>Signup/Login</t>
+  </si>
+  <si>
+    <t>Test new user signup</t>
+  </si>
+  <si>
+    <t>User should be registered successfully</t>
+  </si>
+  <si>
+    <t>Test login with correct credentials</t>
+  </si>
+  <si>
+    <t>User logs in successfully</t>
+  </si>
+  <si>
+    <t>Cart Functionality</t>
+  </si>
+  <si>
+    <t>Add item to cart</t>
+  </si>
+  <si>
+    <t>Item is added and reflected in cart</t>
+  </si>
+  <si>
+    <t>Contact Us</t>
+  </si>
+  <si>
+    <t>Submit form with valid data</t>
+  </si>
+  <si>
+    <t>Confirmation message is shown</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>Search for "Shirt"</t>
+  </si>
+  <si>
+    <t>Matching results should display</t>
+  </si>
+  <si>
+    <t>Footer Navigation</t>
+  </si>
+  <si>
+    <t>Click on "Subscription"</t>
+  </si>
+  <si>
+    <t>Page scrolls and validates email input</t>
+  </si>
+  <si>
+    <t>Invalid Login</t>
+  </si>
+  <si>
+    <t>Expect Error Message for wrong Credentials</t>
+  </si>
+  <si>
+    <t>Attempt to Login with Invalid  Credentials</t>
+  </si>
+  <si>
+    <t>TC09</t>
+  </si>
+  <si>
+    <t>Products &amp; Details</t>
+  </si>
+  <si>
+    <t>View product list, click "View Product"</t>
+  </si>
+  <si>
+    <t>TC10</t>
+  </si>
+  <si>
+    <t>Add Products to Cart</t>
+  </si>
+  <si>
+    <t>Add multiple items, verify in cart</t>
+  </si>
+  <si>
+    <t>Expect "Men's Shirt", Women's Pants and Kid's Shoe in Cart</t>
+  </si>
+  <si>
+    <t>PASSED</t>
+  </si>
+  <si>
+    <t>NOT TESTED</t>
+  </si>
+  <si>
+    <t>Select desired product detailed information</t>
+  </si>
+  <si>
+    <t>VIEWPRODUCT_TEST09.png</t>
+  </si>
+  <si>
+    <t>INVALIDLOGIN_TEST08.png</t>
+  </si>
+  <si>
+    <t>SUBSCRIPTION_TEST07.png</t>
+  </si>
+  <si>
+    <t>SHIRTSEARCH_TEST06.png</t>
+  </si>
+  <si>
+    <t>CONTACTUS_TEST05.png</t>
+  </si>
+  <si>
+    <t>CARTFUNCTION_TEST04.png</t>
+  </si>
+  <si>
+    <t>LOGIN_TEST03.png</t>
+  </si>
+  <si>
+    <t>NEWUSER_TEST02.png</t>
+  </si>
+  <si>
+    <t>HOMEPAGE_TEST01.png</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -45,16 +221,45 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -62,14 +267,178 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -88,7 +457,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Blue Warm">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -96,34 +465,34 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="0E2841"/>
+        <a:srgbClr val="242852"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E8E8E8"/>
+        <a:srgbClr val="ACCBF9"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="156082"/>
+        <a:srgbClr val="4A66AC"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="E97132"/>
+        <a:srgbClr val="629DD1"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="196B24"/>
+        <a:srgbClr val="297FD5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="0F9ED5"/>
+        <a:srgbClr val="7F8FA9"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="A02B93"/>
+        <a:srgbClr val="5AA2AE"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4EA72E"/>
+        <a:srgbClr val="9D90A0"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="467886"/>
+        <a:srgbClr val="9454C3"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607D"/>
+        <a:srgbClr val="3EBBF0"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
@@ -402,12 +771,302 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CE5D67A-17BB-4BA4-93C5-4780DF564567}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+    <col min="5" max="5" width="18.88671875" customWidth="1"/>
+    <col min="6" max="6" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="11"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="14"/>
+    </row>
+    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="G11" r:id="rId1" xr:uid="{690516FB-E90E-4FFD-BF68-E4EC597EEED0}"/>
+    <hyperlink ref="G10" r:id="rId2" xr:uid="{841A48C9-5C61-4C40-A12D-64313E6A405F}"/>
+    <hyperlink ref="G9" r:id="rId3" xr:uid="{A76BB5A1-B433-43BD-ABB7-080D3E6EFD2F}"/>
+    <hyperlink ref="G8" r:id="rId4" xr:uid="{9A3CC7C9-87EF-4A31-88C0-1EEACD096CED}"/>
+    <hyperlink ref="G7" r:id="rId5" xr:uid="{EFE4E245-348B-41BA-852F-40DA76AD3008}"/>
+    <hyperlink ref="G6" r:id="rId6" xr:uid="{890970A9-B809-455D-9840-7FFBF8DE40EB}"/>
+    <hyperlink ref="G5" r:id="rId7" xr:uid="{EC7A1331-EC93-4E8C-912F-849AE8703D7D}"/>
+    <hyperlink ref="G4" r:id="rId8" xr:uid="{40B662ED-8D70-4BE0-BB16-A8AC7EF8CF3C}"/>
+    <hyperlink ref="G3" r:id="rId9" xr:uid="{00EA4EF2-4128-487D-BB93-08A98B412920}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>